<commit_message>
Actualización de tablas y figuras de resultados de informe con datos de CPUE estandarizada (falta revisar redacción de resultados y discusión)
</commit_message>
<xml_diff>
--- a/2022/Tablas cojinoba.xlsx
+++ b/2022/Tablas cojinoba.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/CTP2022/SA_BrotulaCojinovas/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3D323F-B3AF-A641-BFC8-46C62BA50B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ADDABA-54D2-884C-9119-6D96CD50B992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="4780" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{6F3D532C-3ECE-9141-BF46-A5AAD8E273EC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{6F3D532C-3ECE-9141-BF46-A5AAD8E273EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="parámetros" sheetId="1" r:id="rId1"/>
+    <sheet name="cojinoba" sheetId="1" r:id="rId1"/>
     <sheet name="Proyecciones" sheetId="2" r:id="rId2"/>
     <sheet name="TallasXsexo" sheetId="4" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
+    <sheet name="Brotula" sheetId="3" r:id="rId4"/>
+    <sheet name="proyeccionesBrotula" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="182">
   <si>
     <t>[1]</t>
   </si>
@@ -198,9 +199,6 @@
     <t>[52]</t>
   </si>
   <si>
-    <t xml:space="preserve"> E(B_inf)       1.292750e+04           NA           NA  9.4671121  </t>
-  </si>
-  <si>
     <t>Convergence:</t>
   </si>
   <si>
@@ -246,9 +244,6 @@
     <t>C:</t>
   </si>
   <si>
-    <t>33,</t>
-  </si>
-  <si>
     <t>I1:</t>
   </si>
   <si>
@@ -258,18 +253,12 @@
     <t>~</t>
   </si>
   <si>
-    <t>dnorm[log(2),</t>
-  </si>
-  <si>
     <t>2^2]</t>
   </si>
   <si>
     <t>logalpha</t>
   </si>
   <si>
-    <t>dnorm[log(1),</t>
-  </si>
-  <si>
     <t>logbeta</t>
   </si>
   <si>
@@ -429,9 +418,6 @@
     <t>Observed</t>
   </si>
   <si>
-    <t>interval,</t>
-  </si>
-  <si>
     <t>index:</t>
   </si>
   <si>
@@ -577,14 +563,37 @@
   </si>
   <si>
     <t>COJINOBA MOTEADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> E(B_inf)       20296.886052           NA           NA  9.9182228  </t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>X-convergence</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>dnorm[log(2)</t>
+  </si>
+  <si>
+    <t>dnorm[log(1)</t>
+  </si>
+  <si>
+    <t>interval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -639,16 +648,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B33E9725-7D54-7742-8746-76EB83112D1A}">
   <dimension ref="B1:J55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49:H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,838 +990,846 @@
     <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>63.573892200000003</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="3">
+        <v>42370</v>
+      </c>
+      <c r="I5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4">
-        <v>67.672301500000003</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="3">
-        <v>42370</v>
-      </c>
-      <c r="H5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5">
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" t="s">
+      <c r="H9" t="s">
         <v>71</v>
       </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" t="s">
-        <v>75</v>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E10" t="s">
         <v>72</v>
       </c>
       <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>180</v>
+      </c>
+      <c r="H10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
         <v>76</v>
       </c>
-      <c r="G10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" t="s">
+      <c r="F13" t="s">
         <v>77</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" t="s">
-        <v>81</v>
       </c>
       <c r="G13" s="4">
         <v>0.95</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E15" s="5">
-        <v>0.56651390000000001</v>
+        <v>1.2895760000000001</v>
       </c>
       <c r="F15" s="5">
-        <v>0.1290173</v>
+        <v>0.3675834</v>
       </c>
       <c r="G15" s="5">
-        <v>2.4875579999999999</v>
+        <v>4.524159</v>
       </c>
       <c r="H15" s="5">
-        <v>-0.56825369999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+        <v>0.25431340000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E16" s="5">
-        <v>0.50000960000000005</v>
+        <v>0.35419859999999997</v>
       </c>
       <c r="F16" s="5">
-        <v>0.15863240000000001</v>
+        <v>7.0874500000000007E-2</v>
       </c>
       <c r="G16" s="5">
-        <v>1.57603</v>
+        <v>1.7701229999999999</v>
       </c>
       <c r="H16" s="5">
-        <v>-0.69312810000000002</v>
+        <v>-1.0378976</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E17" s="5">
-        <v>8.2817199999999994E-2</v>
+        <v>7.3713399999999998E-2</v>
       </c>
       <c r="F17" s="5">
-        <v>7.0724000000000004E-3</v>
+        <v>4.3782999999999999E-3</v>
       </c>
       <c r="G17" s="5">
-        <v>0.96978640000000005</v>
+        <v>1.241047</v>
       </c>
       <c r="H17" s="5">
-        <v>-2.4911189999999999</v>
+        <v>-2.6075702000000001</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E18" s="5">
-        <v>0.30105150000000003</v>
+        <v>0.281665</v>
       </c>
       <c r="F18" s="5">
-        <v>4.4179900000000001E-2</v>
+        <v>3.8208800000000001E-2</v>
       </c>
       <c r="G18" s="5">
-        <v>2.0514290000000002</v>
+        <v>2.0763600000000002</v>
       </c>
       <c r="H18" s="5">
-        <v>-1.2004739</v>
+        <v>-1.2670368000000001</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E19" s="5">
-        <v>0.18411459999999999</v>
+        <v>0.1546691</v>
       </c>
       <c r="F19" s="5">
-        <v>7.6531000000000004E-3</v>
+        <v>3.6066000000000002E-3</v>
       </c>
       <c r="G19" s="5">
-        <v>4.4293250000000004</v>
+        <v>6.6329750000000001</v>
       </c>
       <c r="H19" s="5">
-        <v>-1.6921968999999999</v>
+        <v>-1.8664670000000001</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E20" s="5">
-        <v>2389.3130000000001</v>
+        <v>2263.3209999999999</v>
       </c>
       <c r="F20" s="5">
-        <v>1034.2792582</v>
+        <v>1419.2789700000001</v>
       </c>
       <c r="G20" s="5">
-        <v>5519.6090000000004</v>
+        <v>3609.3130000000001</v>
       </c>
       <c r="H20" s="5">
-        <v>7.7787611999999999</v>
+        <v>7.7245885000000003</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E21" s="5">
-        <v>59916.43</v>
+        <v>62514.25</v>
       </c>
       <c r="F21" s="5">
-        <v>5703.6613601999998</v>
+        <v>4948.5733446000004</v>
       </c>
       <c r="G21" s="5">
-        <v>629416.5</v>
+        <v>789728.8</v>
       </c>
       <c r="H21" s="5">
-        <v>11.000705999999999</v>
+        <v>11.043149700000001</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E22" s="5">
-        <v>2.5199999999999999E-5</v>
+        <v>3.2499999999999997E-5</v>
       </c>
       <c r="F22" s="5">
-        <v>5.4999999999999999E-6</v>
+        <v>1.47E-5</v>
       </c>
       <c r="G22" s="5">
-        <v>1.166E-4</v>
+        <v>7.1799999999999997E-5</v>
       </c>
       <c r="H22" s="5">
-        <v>-10.587147999999999</v>
+        <v>-10.33389</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E23" s="5">
-        <v>0.55018650000000002</v>
+        <v>0.52341210000000005</v>
       </c>
       <c r="F23" s="5">
-        <v>0.28622609999999998</v>
+        <v>0.217275</v>
       </c>
       <c r="G23" s="5">
-        <v>1.057574</v>
+        <v>1.2608919999999999</v>
       </c>
       <c r="H23" s="5">
-        <v>-0.59749799999999997</v>
+        <v>-0.64738609999999996</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E24" s="5">
-        <v>0.26014589999999999</v>
+        <v>0.13745450000000001</v>
       </c>
       <c r="F24" s="5">
-        <v>0.13913710000000001</v>
+        <v>5.40251E-2</v>
       </c>
       <c r="G24" s="5">
-        <v>0.48639739999999998</v>
+        <v>0.34972170000000002</v>
       </c>
       <c r="H24" s="5">
-        <v>-1.3465125</v>
+        <v>-1.9844619999999999</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E25" s="5">
-        <v>1.0287269999999999</v>
+        <v>1.2078</v>
       </c>
       <c r="F25" s="5">
-        <v>0.60013269999999996</v>
+        <v>0.69571530000000004</v>
       </c>
       <c r="G25" s="5">
-        <v>1.7634080000000001</v>
+        <v>2.0968079999999998</v>
       </c>
       <c r="H25" s="5">
-        <v>2.8321800000000001E-2</v>
+        <v>0.18880060000000001</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E26" s="5">
-        <v>0.14737629999999999</v>
+        <v>0.1772581</v>
       </c>
       <c r="F26" s="5">
-        <v>5.5837600000000001E-2</v>
+        <v>0.110092</v>
       </c>
       <c r="G26" s="5">
-        <v>0.38898129999999997</v>
+        <v>0.28540149999999997</v>
       </c>
       <c r="H26" s="5">
-        <v>-1.9147662000000001</v>
+        <v>-1.7301485999999999</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E27" s="5">
-        <v>0.51437319999999997</v>
+        <v>0.42780109999999999</v>
       </c>
       <c r="F27" s="5">
-        <v>0.25103589999999998</v>
+        <v>0.13693720000000001</v>
       </c>
       <c r="G27" s="5">
-        <v>1.053952</v>
+        <v>1.336479</v>
       </c>
       <c r="H27" s="5">
-        <v>-0.66480629999999996</v>
+        <v>-0.84909699999999999</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E31" s="2">
-        <v>15873.12</v>
+        <v>16071.01</v>
       </c>
       <c r="F31" s="2">
-        <v>1962.4761000000001</v>
+        <v>2024.3456470000001</v>
       </c>
       <c r="G31" s="2">
-        <v>128386.7</v>
+        <v>127585.64986999999</v>
       </c>
       <c r="H31" s="2">
-        <v>9.6723820000000007</v>
+        <v>9.6847720000000006</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E32" s="5">
-        <v>0.15052579999999999</v>
+        <v>0.1408325</v>
       </c>
       <c r="F32" s="5">
-        <v>2.2089999999999999E-2</v>
+        <v>1.9104400000000001E-2</v>
       </c>
       <c r="G32" s="5">
-        <v>1.0257149999999999</v>
+        <v>1.0381800000000001</v>
       </c>
       <c r="H32" s="5">
-        <v>-1.893621</v>
+        <v>-1.9601839999999999</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E33" s="2">
-        <v>2389.3130000000001</v>
+        <v>2263.3209999999999</v>
       </c>
       <c r="F33" s="2">
-        <v>1034.27926</v>
+        <v>1419.2789700000001</v>
       </c>
       <c r="G33" s="2">
-        <v>5519.6090000000004</v>
+        <v>3609.3127599999998</v>
       </c>
       <c r="H33" s="2">
-        <v>7.7787610000000003</v>
+        <v>7.7245889999999999</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E35" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G35" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H35" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E36" s="2">
-        <v>14014.42</v>
+        <v>15512.1</v>
       </c>
       <c r="F36" s="2">
-        <v>2046.0885917999999</v>
+        <v>2011.0896273000001</v>
       </c>
       <c r="G36" s="2">
-        <v>95989.91</v>
+        <v>119649.2</v>
       </c>
       <c r="H36" s="2">
-        <v>9.5478419999999993</v>
+        <v>9.6493760000000002</v>
       </c>
       <c r="I36" s="5">
-        <v>-0.13262778</v>
+        <v>-3.6030520000000003E-2</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E37" s="5">
-        <v>0.1580857</v>
+        <v>0.1430707</v>
       </c>
       <c r="F37" s="5">
-        <v>2.5649100000000001E-2</v>
+        <v>1.99626E-2</v>
       </c>
       <c r="G37" s="5">
-        <v>0.97434710000000002</v>
+        <v>1.025379</v>
       </c>
       <c r="H37" s="5">
-        <v>-1.8446180000000001</v>
+        <v>-1.9444159999999999</v>
       </c>
       <c r="I37" s="5">
-        <v>4.7821780000000001E-2</v>
+        <v>1.5644000000000002E-2</v>
       </c>
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E38" s="2">
-        <v>2229.5309999999999</v>
+        <v>2220.5790000000002</v>
       </c>
       <c r="F38" s="2">
-        <v>977.10993719999999</v>
+        <v>1400.9635785999999</v>
       </c>
       <c r="G38" s="2">
-        <v>5087.2560000000003</v>
+        <v>3519.6990000000001</v>
       </c>
       <c r="H38" s="2">
-        <v>7.7095469999999997</v>
+        <v>7.7055230000000003</v>
       </c>
       <c r="I38" s="5">
-        <v>-7.1666209999999994E-2</v>
+        <v>-1.924822E-2</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D40" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E40" s="4">
         <v>0.95</v>
       </c>
       <c r="F40" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H40" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E41" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E42" s="2">
-        <v>10989.34</v>
+        <v>8437.2260143999993</v>
       </c>
       <c r="F42" s="2">
-        <v>2186.1565928999999</v>
+        <v>3484.6711777</v>
       </c>
       <c r="G42" s="2">
-        <v>55241.077367999998</v>
+        <v>20428.55</v>
       </c>
       <c r="H42" s="5">
-        <v>9.3046811999999992</v>
+        <v>9.0404090000000004</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E43" s="5">
-        <v>0.17274909999999999</v>
+        <v>0.22266559999999999</v>
       </c>
       <c r="F43" s="5">
-        <v>2.2040400000000002E-2</v>
+        <v>5.2823299999999997E-2</v>
       </c>
       <c r="G43" s="5">
-        <v>1.3539760000000001</v>
+        <v>0.9386004</v>
       </c>
       <c r="H43" s="5">
-        <v>-1.7559151</v>
+        <v>-1.502084</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E44" s="5">
-        <v>0.7841456</v>
+        <v>0.54391239999999996</v>
       </c>
       <c r="F44" s="5">
-        <v>5.9922499999999997E-2</v>
+        <v>6.3513899999999998E-2</v>
       </c>
       <c r="G44" s="5">
-        <v>10.261322</v>
+        <v>4.6578929999999996</v>
       </c>
       <c r="H44" s="5">
-        <v>-0.2431606</v>
+        <v>-0.60896700000000004</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E45" s="5">
-        <v>1.0927560000000001</v>
+        <v>1.5563324000000001</v>
       </c>
       <c r="F45" s="5">
-        <v>4.7989499999999997E-2</v>
+        <v>0.13952120000000001</v>
       </c>
       <c r="G45" s="5">
-        <v>24.882818</v>
+        <v>17.360589999999998</v>
       </c>
       <c r="H45" s="5">
-        <v>8.8702600000000006E-2</v>
+        <v>0.442332</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" s="5"/>
@@ -1818,177 +1839,190 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E47" s="4">
         <v>0.95</v>
       </c>
       <c r="F47" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G47" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H47" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E48" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F48" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G48" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E49" s="2">
-        <v>11034.14</v>
+        <v>8554.7859793999996</v>
       </c>
       <c r="F49" s="2">
-        <v>1833.1537103000001</v>
+        <v>3141.5881727000001</v>
       </c>
       <c r="G49" s="2">
-        <v>66416.842967999997</v>
+        <v>23295.339532000002</v>
       </c>
       <c r="H49" s="5">
-        <v>9.3087494999999993</v>
+        <v>9.0542461999999997</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E50" s="5">
-        <v>0.17177719999999999</v>
+        <v>0.2223753</v>
       </c>
       <c r="F50" s="5">
-        <v>1.67204E-2</v>
+        <v>3.2785500000000002E-2</v>
       </c>
       <c r="G50" s="5">
-        <v>1.7647520000000001</v>
+        <v>1.5083139999999999</v>
       </c>
       <c r="H50" s="5">
-        <v>-1.7615567999999999</v>
+        <v>-1.5033886999999999</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E51" s="5">
-        <v>0.78734219999999999</v>
+        <v>0.55149099999999995</v>
       </c>
       <c r="F51" s="5">
-        <v>5.4112300000000002E-2</v>
+        <v>5.8204899999999997E-2</v>
       </c>
       <c r="G51" s="5">
-        <v>11.455945</v>
+        <v>5.2253759999999998</v>
       </c>
       <c r="H51" s="5">
-        <v>-0.23909230000000001</v>
+        <v>-0.59512969999999998</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E52" s="5">
-        <v>1.086608</v>
+        <v>1.5543035000000001</v>
       </c>
       <c r="F52" s="5">
-        <v>4.0939700000000002E-2</v>
+        <v>9.8141800000000001E-2</v>
       </c>
       <c r="G52" s="5">
-        <v>28.840394</v>
+        <v>24.616004</v>
       </c>
       <c r="H52" s="5">
-        <v>8.3060999999999996E-2</v>
+        <v>0.44102750000000002</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E53" s="2">
-        <v>1899.115</v>
+        <v>1913.0460731000001</v>
       </c>
       <c r="F53" s="2">
-        <v>318.23974129999999</v>
+        <v>292.13340540000002</v>
       </c>
       <c r="G53" s="2">
-        <v>11333.089857000001</v>
+        <v>12527.650758</v>
       </c>
       <c r="H53" s="5">
-        <v>7.5491434999999996</v>
+        <v>7.5564520999999996</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E54" s="2">
-        <v>12927.5</v>
+        <v>9558.4673456</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H54" s="5">
-        <v>9.4671120999999996</v>
+        <v>9.1651827000000008</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>53</v>
+      <c r="C55" s="2"/>
+      <c r="D55" t="s">
+        <v>123</v>
+      </c>
+      <c r="E55" s="9">
+        <v>12927.5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>124</v>
+      </c>
+      <c r="G55" t="s">
+        <v>124</v>
+      </c>
+      <c r="H55">
+        <v>9.4671120999999996</v>
       </c>
     </row>
   </sheetData>
@@ -2000,33 +2034,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D4345A-66A5-2C43-BE69-215639B4CB0F}">
   <dimension ref="B1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B1" s="8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C1" s="8"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E3">
         <v>1997</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G3">
         <v>2021</v>
@@ -2034,19 +2068,19 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E4">
         <v>1989</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G4">
         <v>2022</v>
@@ -2057,16 +2091,16 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F6">
         <v>2023</v>
@@ -2074,13 +2108,13 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E7">
         <v>2023</v>
@@ -2088,22 +2122,22 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F8">
         <v>2022</v>
       </c>
       <c r="G8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H8">
         <v>2023</v>
@@ -2114,31 +2148,31 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" t="s">
         <v>143</v>
       </c>
-      <c r="D11" t="s">
+      <c r="I11" t="s">
         <v>144</v>
-      </c>
-      <c r="E11" t="s">
-        <v>145</v>
-      </c>
-      <c r="F11" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H11" t="s">
-        <v>148</v>
-      </c>
-      <c r="I11" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
@@ -2146,34 +2180,34 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F12">
-        <v>1891.4</v>
+        <v>1893</v>
       </c>
       <c r="G12">
-        <v>11084.9</v>
+        <v>8676.1</v>
       </c>
       <c r="H12">
-        <v>0.17100000000000001</v>
+        <v>0.219</v>
       </c>
       <c r="I12">
-        <v>0.69799999999999995</v>
+        <v>0.54</v>
       </c>
       <c r="J12">
-        <v>1.081</v>
+        <v>1.532</v>
       </c>
       <c r="K12">
-        <v>0.5</v>
+        <v>1.4</v>
       </c>
       <c r="L12">
-        <v>-0.5</v>
+        <v>-1.4</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
@@ -2181,31 +2215,31 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F13">
-        <v>1899.1</v>
+        <v>1913</v>
       </c>
       <c r="G13">
-        <v>11078.7</v>
+        <v>8654</v>
       </c>
       <c r="H13">
-        <v>0.17199999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="I13">
-        <v>0.69799999999999995</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="J13">
-        <v>1.087</v>
+        <v>1.554</v>
       </c>
       <c r="K13">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2216,34 +2250,34 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F14">
-        <v>1758.5</v>
+        <v>1275.3</v>
       </c>
       <c r="G14">
-        <v>11219.4</v>
+        <v>9306.7000000000007</v>
       </c>
       <c r="H14">
-        <v>0.158</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="I14">
-        <v>0.70699999999999996</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <v>1.7</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L14">
-        <v>-8</v>
+        <v>-35.700000000000003</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
@@ -2251,30 +2285,30 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15">
+        <v>151</v>
+      </c>
+      <c r="F15">
         <v>2.1</v>
       </c>
-      <c r="F15">
-        <v>12979.9</v>
-      </c>
       <c r="G15">
+        <v>10612.7</v>
+      </c>
+      <c r="H15">
         <v>0</v>
       </c>
-      <c r="H15">
-        <v>0.81799999999999995</v>
-      </c>
       <c r="I15">
-        <v>1E-3</v>
+        <v>0.66</v>
       </c>
       <c r="J15">
-        <v>17.600000000000001</v>
+        <v>2E-3</v>
       </c>
       <c r="K15">
+        <v>24.1</v>
+      </c>
+      <c r="L15">
         <v>-99.9</v>
       </c>
     </row>
@@ -2283,31 +2317,31 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E16" s="4">
         <v>0.25</v>
       </c>
       <c r="F16">
-        <v>1452</v>
+        <v>1470.9</v>
       </c>
       <c r="G16">
-        <v>11526</v>
+        <v>9106.4</v>
       </c>
       <c r="H16">
-        <v>0.129</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="I16">
-        <v>0.72599999999999998</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="J16">
-        <v>0.81499999999999995</v>
+        <v>1.1659999999999999</v>
       </c>
       <c r="K16">
-        <v>4.5</v>
+        <v>6.4</v>
       </c>
       <c r="L16">
         <v>-25</v>
@@ -2318,31 +2352,31 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E17" s="4">
         <v>0.25</v>
       </c>
       <c r="F17">
-        <v>2329.1</v>
+        <v>2333.1999999999998</v>
       </c>
       <c r="G17">
-        <v>10649.2</v>
+        <v>8224.7000000000007</v>
       </c>
       <c r="H17">
-        <v>0.215</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="I17">
-        <v>0.67100000000000004</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="J17">
-        <v>1.3580000000000001</v>
+        <v>1.9430000000000001</v>
       </c>
       <c r="K17">
-        <v>-3.5</v>
+        <v>-3.9</v>
       </c>
       <c r="L17">
         <v>25</v>
@@ -2353,34 +2387,34 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D18" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F18">
-        <v>1758.5</v>
+        <v>1275.3</v>
       </c>
       <c r="G18">
-        <v>11219.4</v>
+        <v>9306.7000000000007</v>
       </c>
       <c r="H18">
-        <v>0.158</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="I18">
-        <v>0.70699999999999996</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="K18">
-        <v>1.7</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L18">
-        <v>-8</v>
+        <v>-35.700000000000003</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
@@ -2391,37 +2425,37 @@
         <v>0.95</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D20" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" t="s">
+        <v>164</v>
+      </c>
+      <c r="G21" t="s">
+        <v>165</v>
+      </c>
+      <c r="H21" t="s">
         <v>166</v>
-      </c>
-      <c r="D21" t="s">
-        <v>167</v>
-      </c>
-      <c r="E21" t="s">
-        <v>168</v>
-      </c>
-      <c r="F21" t="s">
-        <v>169</v>
-      </c>
-      <c r="G21" t="s">
-        <v>170</v>
-      </c>
-      <c r="H21" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
@@ -2429,31 +2463,31 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E22" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F22">
-        <v>786</v>
+        <v>880</v>
       </c>
       <c r="G22">
-        <v>4551.5</v>
+        <v>4072</v>
       </c>
       <c r="H22">
-        <v>1488.2</v>
+        <v>2815.6</v>
       </c>
       <c r="I22">
-        <v>82567.3</v>
+        <v>26735.1</v>
       </c>
       <c r="J22">
-        <v>1.4E-2</v>
+        <v>0.03</v>
       </c>
       <c r="K22">
-        <v>2.048</v>
+        <v>1.577</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
@@ -2461,31 +2495,31 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F23">
-        <v>318.2</v>
+        <v>292.10000000000002</v>
       </c>
       <c r="G23">
-        <v>11333.1</v>
+        <v>12527.7</v>
       </c>
       <c r="H23">
-        <v>1561</v>
+        <v>2622.2</v>
       </c>
       <c r="I23">
-        <v>78626.7</v>
+        <v>28560.2</v>
       </c>
       <c r="J23">
-        <v>8.0000000000000002E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="K23">
-        <v>3.7410000000000001</v>
+        <v>4.67</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
@@ -2493,31 +2527,31 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F24">
-        <v>291.5</v>
+        <v>181.3</v>
       </c>
       <c r="G24">
-        <v>10607</v>
+        <v>8969.9</v>
       </c>
       <c r="H24">
-        <v>1619.9</v>
+        <v>3166.5</v>
       </c>
       <c r="I24">
-        <v>77705.2</v>
+        <v>27352.9</v>
       </c>
       <c r="J24">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="K24">
-        <v>3.4430000000000001</v>
+        <v>3.004</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
@@ -2525,28 +2559,28 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D25" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E25">
         <v>0.3</v>
       </c>
       <c r="F25">
-        <v>14.1</v>
+        <v>17</v>
       </c>
       <c r="G25">
-        <v>2436.9</v>
+        <v>4269.2</v>
       </c>
       <c r="H25">
-        <v>69134.3</v>
+        <v>26382</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25">
-        <v>4.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
@@ -2554,31 +2588,31 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E26" s="4">
         <v>0.25</v>
       </c>
       <c r="F26">
-        <v>235.2</v>
+        <v>213.7</v>
       </c>
       <c r="G26">
-        <v>8965.2000000000007</v>
+        <v>10124.1</v>
       </c>
       <c r="H26">
-        <v>1751.9</v>
+        <v>2996.9</v>
       </c>
       <c r="I26">
-        <v>75830.899999999994</v>
+        <v>27670.6</v>
       </c>
       <c r="J26">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="K26">
-        <v>2.806</v>
+        <v>3.5019999999999998</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
@@ -2586,31 +2620,31 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D27" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E27" s="4">
         <v>0.25</v>
       </c>
       <c r="F27">
-        <v>403.3</v>
+        <v>374</v>
       </c>
       <c r="G27">
-        <v>13448.6</v>
+        <v>14555</v>
       </c>
       <c r="H27">
-        <v>1388.1</v>
+        <v>2282.5</v>
       </c>
       <c r="I27">
-        <v>81700.5</v>
+        <v>29636</v>
       </c>
       <c r="J27">
-        <v>0.01</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="K27">
-        <v>4.6769999999999996</v>
+        <v>5.8369999999999997</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
@@ -2618,31 +2652,31 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D28" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E28" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F28">
-        <v>291.5</v>
+        <v>181.3</v>
       </c>
       <c r="G28">
-        <v>10607</v>
+        <v>8969.9</v>
       </c>
       <c r="H28">
-        <v>1619.9</v>
+        <v>3166.5</v>
       </c>
       <c r="I28">
-        <v>77705.2</v>
+        <v>27352.9</v>
       </c>
       <c r="J28">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="K28">
-        <v>3.4430000000000001</v>
+        <v>3.004</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
@@ -2653,31 +2687,31 @@
         <v>0.95</v>
       </c>
       <c r="C30" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D30" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D31" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E31" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F31" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
@@ -2685,25 +2719,25 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D32" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E32" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F32">
-        <v>3.4000000000000002E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="G32">
-        <v>14.268000000000001</v>
+        <v>5.9489999999999998</v>
       </c>
       <c r="H32">
-        <v>3.5000000000000003E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="I32">
-        <v>33.875</v>
+        <v>26.936</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
@@ -2711,25 +2745,25 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E33" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F33">
-        <v>3.5999999999999997E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G33">
-        <v>13.477</v>
+        <v>6.0209999999999999</v>
       </c>
       <c r="H33">
-        <v>2.3E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="I33">
-        <v>51.015999999999998</v>
+        <v>59.085000000000001</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
@@ -2737,25 +2771,25 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F34">
-        <v>3.6999999999999998E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="G34">
-        <v>13.404</v>
+        <v>6.1219999999999999</v>
       </c>
       <c r="H34">
-        <v>2.1000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I34">
-        <v>46.95</v>
+        <v>38.014000000000003</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
@@ -2763,22 +2797,22 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E35">
-        <v>5.1999999999999998E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="F35">
-        <v>12.827999999999999</v>
+        <v>6.4859999999999998</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
-        <v>5.0999999999999997E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
@@ -2786,25 +2820,25 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E36" s="4">
         <v>0.25</v>
       </c>
       <c r="F36">
-        <v>0.04</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="G36">
-        <v>13.26</v>
+        <v>6.085</v>
       </c>
       <c r="H36">
-        <v>1.7000000000000001E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="I36">
-        <v>38.262</v>
+        <v>44.314</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
@@ -2812,25 +2846,25 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E37" s="4">
         <v>0.25</v>
       </c>
       <c r="F37">
-        <v>3.3000000000000002E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="G37">
-        <v>13.728999999999999</v>
+        <v>5.9880000000000004</v>
       </c>
       <c r="H37">
-        <v>2.9000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="I37">
-        <v>63.77</v>
+        <v>73.856999999999999</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
@@ -2838,25 +2872,25 @@
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E38" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F38">
-        <v>3.6999999999999998E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="G38">
-        <v>13.404</v>
+        <v>6.1219999999999999</v>
       </c>
       <c r="H38">
-        <v>2.1000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I38">
-        <v>46.95</v>
+        <v>38.014000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2876,13 +2910,13 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="L1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
@@ -3659,14 +3693,1751 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B76C5BE-B141-DC46-A03D-2776B1E3A93B}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="H11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.43681019999999998</v>
+      </c>
+      <c r="F13" s="5">
+        <v>9.8831000000000002E-2</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1.9306000000000001</v>
+      </c>
+      <c r="H13" s="5">
+        <v>-0.82825649999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0.5455605</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.23007849999999999</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1.2936289999999999</v>
+      </c>
+      <c r="H14" s="5">
+        <v>-0.60594150000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.60270990000000002</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.30859199999999998</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1.1771499999999999</v>
+      </c>
+      <c r="H15" s="5">
+        <v>-0.50631930000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1.3070809999999999</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.72887880000000005</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2.3439580000000002</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.2677966</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="5">
+        <v>7.7491589999999997</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1.2787056999999999</v>
+      </c>
+      <c r="G17" s="5">
+        <v>46.961129999999997</v>
+      </c>
+      <c r="H17" s="5">
+        <v>2.0475843</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="10">
+        <v>5870.63</v>
+      </c>
+      <c r="F18" s="10">
+        <v>2999.7395669000002</v>
+      </c>
+      <c r="G18" s="10">
+        <v>11489.1</v>
+      </c>
+      <c r="H18" s="10">
+        <v>8.6777172999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="10">
+        <v>25440.52</v>
+      </c>
+      <c r="F19" s="10">
+        <v>7851.1418783999998</v>
+      </c>
+      <c r="G19" s="10">
+        <v>82436.42</v>
+      </c>
+      <c r="H19" s="10">
+        <v>10.1440985</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1.6099999999999998E-5</v>
+      </c>
+      <c r="F20" s="5">
+        <v>4.5000000000000001E-6</v>
+      </c>
+      <c r="G20" s="5">
+        <v>5.7200000000000001E-5</v>
+      </c>
+      <c r="H20" s="5">
+        <v>-11.037082099999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.92222249999999995</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.83433029999999997</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1.019374</v>
+      </c>
+      <c r="H21" s="5">
+        <v>-8.0968700000000005E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.50697729999999996</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.3156429</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.81429359999999995</v>
+      </c>
+      <c r="H22" s="5">
+        <v>-0.67928909999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.5897348</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.37086449999999999</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.93777410000000005</v>
+      </c>
+      <c r="H23" s="5">
+        <v>-0.52808239999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.22145290000000001</v>
+      </c>
+      <c r="F24" s="5">
+        <v>6.6678200000000007E-2</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.73549330000000002</v>
+      </c>
+      <c r="H24" s="5">
+        <v>-1.5075455</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.32173600000000002</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.18616750000000001</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.55602640000000003</v>
+      </c>
+      <c r="H25" s="5">
+        <v>-1.1340239000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="11">
+        <v>8982.8081736000004</v>
+      </c>
+      <c r="F29" s="11">
+        <v>2866.7529334999999</v>
+      </c>
+      <c r="G29" s="11">
+        <v>28147.121343999999</v>
+      </c>
+      <c r="H29" s="11">
+        <v>9.1030677999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.65354060000000003</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.36443940000000002</v>
+      </c>
+      <c r="G30" s="5">
+        <v>1.1719790000000001</v>
+      </c>
+      <c r="H30" s="5">
+        <v>-0.42535060000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="11">
+        <v>5870.6301297</v>
+      </c>
+      <c r="F31" s="11">
+        <v>2999.7395669000002</v>
+      </c>
+      <c r="G31" s="11">
+        <v>11489.096754</v>
+      </c>
+      <c r="H31" s="11">
+        <v>8.6777172999999994</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="11">
+        <v>7720.4558164</v>
+      </c>
+      <c r="F34" s="11">
+        <v>2382.238398</v>
+      </c>
+      <c r="G34" s="11">
+        <v>25020.769568</v>
+      </c>
+      <c r="H34" s="11">
+        <v>8.9516287000000005</v>
+      </c>
+      <c r="I34" s="11">
+        <v>-0.163507491</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.65736090000000003</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.36984460000000002</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1.1683920000000001</v>
+      </c>
+      <c r="H35" s="5">
+        <v>-0.41952210000000001</v>
+      </c>
+      <c r="I35" s="5">
+        <v>5.8115229999999999E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="11">
+        <v>5079.9485238999996</v>
+      </c>
+      <c r="F36" s="11">
+        <v>2531.6535269000001</v>
+      </c>
+      <c r="G36" s="11">
+        <v>10193.289379</v>
+      </c>
+      <c r="H36" s="11">
+        <v>8.5330563999999995</v>
+      </c>
+      <c r="I36" s="11">
+        <v>-0.15564756299999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" t="s">
+        <v>110</v>
+      </c>
+      <c r="H38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="2">
+        <v>10761.4</v>
+      </c>
+      <c r="F40" s="2">
+        <v>2904.1085207000001</v>
+      </c>
+      <c r="G40" s="2">
+        <v>39877.18</v>
+      </c>
+      <c r="H40" s="12">
+        <v>9.2837206000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="12">
+        <v>5.6084999999999998E-3</v>
+      </c>
+      <c r="F41" s="12">
+        <v>1.3872000000000001E-3</v>
+      </c>
+      <c r="G41" s="12">
+        <v>2.26746E-2</v>
+      </c>
+      <c r="H41" s="12">
+        <v>-5.1834736000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="12">
+        <v>1.3938809999999999</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0.83275120000000002</v>
+      </c>
+      <c r="G42" s="12">
+        <v>2.3331149999999998</v>
+      </c>
+      <c r="H42" s="12">
+        <v>0.3320919</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" s="12">
+        <v>8.5318000000000008E-3</v>
+      </c>
+      <c r="F43" s="12">
+        <v>2.9621999999999999E-3</v>
+      </c>
+      <c r="G43" s="12">
+        <v>2.4573899999999999E-2</v>
+      </c>
+      <c r="H43" s="12">
+        <v>-4.7639515000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="F45" t="s">
+        <v>78</v>
+      </c>
+      <c r="G45" t="s">
+        <v>110</v>
+      </c>
+      <c r="H45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" t="s">
+        <v>80</v>
+      </c>
+      <c r="F46" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="2">
+        <v>14051.911881</v>
+      </c>
+      <c r="F47" s="2">
+        <v>3713.2220726999999</v>
+      </c>
+      <c r="G47" s="2">
+        <v>53176.52</v>
+      </c>
+      <c r="H47" s="12">
+        <v>9.5505136999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="5">
+        <v>5.1570000000000001E-3</v>
+      </c>
+      <c r="F48" s="5">
+        <v>1.0923E-3</v>
+      </c>
+      <c r="G48" s="5">
+        <v>2.4348100000000001E-2</v>
+      </c>
+      <c r="H48" s="5">
+        <v>-5.2674013999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" s="5">
+        <v>1.8200879999999999</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0.81998439999999995</v>
+      </c>
+      <c r="G49" s="5">
+        <v>4.039981</v>
+      </c>
+      <c r="H49" s="5">
+        <v>0.59888509999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" t="s">
+        <v>121</v>
+      </c>
+      <c r="E50" s="5">
+        <v>7.8449999999999995E-3</v>
+      </c>
+      <c r="F50" s="5">
+        <v>2.2181000000000002E-3</v>
+      </c>
+      <c r="G50" s="5">
+        <v>2.7746099999999999E-2</v>
+      </c>
+      <c r="H50" s="5">
+        <v>-4.8478792999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="5">
+        <v>79.499480000000005</v>
+      </c>
+      <c r="F51" s="5">
+        <v>22.089452000000001</v>
+      </c>
+      <c r="G51" s="5">
+        <v>286.11700000000002</v>
+      </c>
+      <c r="H51" s="5">
+        <v>4.3757504999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="2">
+        <v>20296.886052000002</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H52" s="5">
+        <v>9.9182228000000006</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365D0E9D-B77E-BA40-87AF-DAB2892512B7}">
+  <dimension ref="B2:L37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2">
+        <v>1997</v>
+      </c>
+      <c r="F2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3">
+        <v>1978</v>
+      </c>
+      <c r="F3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7">
+        <v>2022</v>
+      </c>
+      <c r="G7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="G11">
+        <v>16035.2</v>
+      </c>
+      <c r="H11">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I11">
+        <v>1.7849999999999999</v>
+      </c>
+      <c r="J11">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="K11">
+        <v>14.1</v>
+      </c>
+      <c r="L11">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12">
+        <v>79.5</v>
+      </c>
+      <c r="G12">
+        <v>16741.099999999999</v>
+      </c>
+      <c r="H12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I12">
+        <v>1.8640000000000001</v>
+      </c>
+      <c r="J12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K12">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13">
+        <v>7869.1</v>
+      </c>
+      <c r="G13">
+        <v>10255.200000000001</v>
+      </c>
+      <c r="H13">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="I13">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>-27</v>
+      </c>
+      <c r="L13">
+        <v>12647</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14">
+        <v>0.1</v>
+      </c>
+      <c r="F14">
+        <v>16806.3</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1.871</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K14">
+        <v>-99.9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F15">
+        <v>59.7</v>
+      </c>
+      <c r="G15">
+        <v>16757.400000000001</v>
+      </c>
+      <c r="H15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I15">
+        <v>1.865</v>
+      </c>
+      <c r="J15">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K15">
+        <v>19.3</v>
+      </c>
+      <c r="L15">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F16">
+        <v>99.3</v>
+      </c>
+      <c r="G16">
+        <v>16724.8</v>
+      </c>
+      <c r="H16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I16">
+        <v>1.8620000000000001</v>
+      </c>
+      <c r="J16">
+        <v>0.01</v>
+      </c>
+      <c r="K16">
+        <v>19</v>
+      </c>
+      <c r="L16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17">
+        <v>7869.1</v>
+      </c>
+      <c r="G17">
+        <v>10255.200000000001</v>
+      </c>
+      <c r="H17">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="I17">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>-27</v>
+      </c>
+      <c r="L17">
+        <v>12647</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21">
+        <v>36.9</v>
+      </c>
+      <c r="G21">
+        <v>115</v>
+      </c>
+      <c r="H21">
+        <v>4168.1000000000004</v>
+      </c>
+      <c r="I21">
+        <v>61689.3</v>
+      </c>
+      <c r="J21">
+        <v>1E-3</v>
+      </c>
+      <c r="K21">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22">
+        <v>22.1</v>
+      </c>
+      <c r="G22">
+        <v>286.10000000000002</v>
+      </c>
+      <c r="H22">
+        <v>4307.3999999999996</v>
+      </c>
+      <c r="I22">
+        <v>65065.2</v>
+      </c>
+      <c r="J22">
+        <v>1E-3</v>
+      </c>
+      <c r="K22">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23">
+        <v>2753.1</v>
+      </c>
+      <c r="G23">
+        <v>22491.8</v>
+      </c>
+      <c r="H23">
+        <v>1531.8</v>
+      </c>
+      <c r="I23">
+        <v>68659.5</v>
+      </c>
+      <c r="J23">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="K23">
+        <v>4.5529999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0.3</v>
+      </c>
+      <c r="G24">
+        <v>4338.8999999999996</v>
+      </c>
+      <c r="H24">
+        <v>65097.9</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F25">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G25">
+        <v>214.8</v>
+      </c>
+      <c r="H25">
+        <v>4315.3</v>
+      </c>
+      <c r="I25">
+        <v>65073.2</v>
+      </c>
+      <c r="J25">
+        <v>1E-3</v>
+      </c>
+      <c r="K25">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F26">
+        <v>27.6</v>
+      </c>
+      <c r="G26">
+        <v>357.3</v>
+      </c>
+      <c r="H26">
+        <v>4299.6000000000004</v>
+      </c>
+      <c r="I26">
+        <v>65057.2</v>
+      </c>
+      <c r="J26">
+        <v>1E-3</v>
+      </c>
+      <c r="K26">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27">
+        <v>2753.1</v>
+      </c>
+      <c r="G27">
+        <v>22491.8</v>
+      </c>
+      <c r="H27">
+        <v>1531.8</v>
+      </c>
+      <c r="I27">
+        <v>68659.5</v>
+      </c>
+      <c r="J27">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="K27">
+        <v>4.5529999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31">
+        <v>0.747</v>
+      </c>
+      <c r="G31">
+        <v>4.266</v>
+      </c>
+      <c r="H31">
+        <v>2E-3</v>
+      </c>
+      <c r="I31">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32">
+        <v>0.76</v>
+      </c>
+      <c r="G32">
+        <v>4.569</v>
+      </c>
+      <c r="H32">
+        <v>1E-3</v>
+      </c>
+      <c r="I32">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F33">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G33">
+        <v>3.9129999999999998</v>
+      </c>
+      <c r="H33">
+        <v>0.18</v>
+      </c>
+      <c r="I33">
+        <v>5.5410000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="F34">
+        <v>4.585</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F35">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="G35">
+        <v>4.5730000000000004</v>
+      </c>
+      <c r="H35">
+        <v>1E-3</v>
+      </c>
+      <c r="I35">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F36">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="G36">
+        <v>4.5650000000000004</v>
+      </c>
+      <c r="H36">
+        <v>2E-3</v>
+      </c>
+      <c r="I36">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="G37">
+        <v>3.9129999999999998</v>
+      </c>
+      <c r="H37">
+        <v>0.18</v>
+      </c>
+      <c r="I37">
+        <v>5.5410000000000004</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>